<commit_message>
add hospital table script.
</commit_message>
<xml_diff>
--- a/Hospital Management System/Documents/DataDictionary.xlsx
+++ b/Hospital Management System/Documents/DataDictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8580"/>
+    <workbookView windowWidth="18345" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="hms_config" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="62">
   <si>
     <t>Table Name</t>
   </si>
@@ -158,6 +158,48 @@
   </si>
   <si>
     <t>deleteop</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>hospitalid</t>
+  </si>
+  <si>
+    <t>hospitalcode</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hospital </t>
+  </si>
+  <si>
+    <t>hospital name</t>
+  </si>
+  <si>
+    <t>shortname</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>databasename</t>
+  </si>
+  <si>
+    <t>connectionstring</t>
+  </si>
+  <si>
+    <t>varchar(max)</t>
+  </si>
+  <si>
+    <t>custome</t>
+  </si>
+  <si>
+    <t>hospitallogo</t>
   </si>
 </sst>
 </file>
@@ -170,7 +212,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,13 +223,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -641,148 +676,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1108,24 +1143,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="19.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="22.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="19.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="22.8857142857143" customWidth="1"/>
     <col min="3" max="3" width="16.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="11.4444444444444" customWidth="1"/>
-    <col min="5" max="5" width="13.7777777777778" customWidth="1"/>
-    <col min="6" max="6" width="18.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="33.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="11.447619047619" customWidth="1"/>
+    <col min="5" max="5" width="13.7809523809524" customWidth="1"/>
+    <col min="6" max="6" width="18.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="33.447619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.4" spans="1:7">
+    <row r="1" ht="23.25" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1770,6 +1805,159 @@
       </c>
       <c r="E47" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>255</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add employee repository and enum class.
</commit_message>
<xml_diff>
--- a/Hospital Management System/Documents/DataDictionary.xlsx
+++ b/Hospital Management System/Documents/DataDictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18345" windowHeight="7650"/>
+    <workbookView windowWidth="23040" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="hms_config" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="80">
   <si>
     <t>Table Name</t>
   </si>
@@ -200,6 +200,60 @@
   </si>
   <si>
     <t>hospitallogo</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>departmentid</t>
+  </si>
+  <si>
+    <t>fk_hospital</t>
+  </si>
+  <si>
+    <t>departmentcode</t>
+  </si>
+  <si>
+    <t>departmentname</t>
+  </si>
+  <si>
+    <t>discription</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>empid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no </t>
+  </si>
+  <si>
+    <t>fk_dipartment</t>
+  </si>
+  <si>
+    <t>emptype</t>
+  </si>
+  <si>
+    <t>empcode</t>
+  </si>
+  <si>
+    <t>empname</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>qualification</t>
+  </si>
+  <si>
+    <t>job specification</t>
   </si>
 </sst>
 </file>
@@ -1143,24 +1197,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="19.552380952381" customWidth="1"/>
-    <col min="2" max="2" width="22.8857142857143" customWidth="1"/>
+    <col min="1" max="1" width="19.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="22.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="16.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="11.447619047619" customWidth="1"/>
-    <col min="5" max="5" width="13.7809523809524" customWidth="1"/>
-    <col min="6" max="6" width="18.552380952381" customWidth="1"/>
-    <col min="7" max="7" width="33.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="11.4444444444444" customWidth="1"/>
+    <col min="5" max="5" width="13.7777777777778" customWidth="1"/>
+    <col min="6" max="6" width="18.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="33.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25" spans="1:7">
+    <row r="1" ht="23.4" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1957,6 +2011,269 @@
         <v>13</v>
       </c>
       <c r="E58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64">
+        <v>255</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" t="s">
+        <v>75</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75">
+        <v>20</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76">
+        <v>255</v>
+      </c>
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78">
+        <v>15</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79">
+        <v>50</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>69</v>
+      </c>
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80">
+        <v>255</v>
+      </c>
+      <c r="E80" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81">
+        <v>255</v>
+      </c>
+      <c r="E81" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>